<commit_message>
working on vaporize_theia.py mg/si and mg/al
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data Fegley 2023.xlsx
+++ b/data/MAGMA_Thermodynamic_Data Fegley 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\PycharmProjects\MAGMApy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/MAGMApy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8B5C2E-F479-4B43-868E-43D32A73F155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8A3A0C-D5F6-8E4D-AE96-1402079B98E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20865" yWindow="855" windowWidth="17070" windowHeight="18585" activeTab="3" xr2:uid="{A66FC4F3-F169-E14C-B2AF-C9A0F5AF27FB}"/>
+    <workbookView xWindow="1540" yWindow="1100" windowWidth="31420" windowHeight="21240" activeTab="3" xr2:uid="{A66FC4F3-F169-E14C-B2AF-C9A0F5AF27FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1134,9 +1134,9 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>2655395.9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>-46992</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>-44992</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>-49586</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>-153255</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>-95362</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>-40286</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>36404</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>63948</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>204359</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>200903</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1493,9 +1493,9 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2443,12 +2443,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>162</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>163</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>165</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>167</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -3458,12 +3458,12 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>172</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3508,10 +3508,10 @@
         <v>174</v>
       </c>
       <c r="C3">
-        <v>-18.8489</v>
+        <v>-12.8489</v>
       </c>
       <c r="D3">
-        <v>64286.3</v>
+        <v>43367.3</v>
       </c>
       <c r="E3">
         <f>-2655400</f>
@@ -3521,7 +3521,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>95</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
work in progress on vaporize_theia.py
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data Fegley 2023.xlsx
+++ b/data/MAGMA_Thermodynamic_Data Fegley 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/MAGMApy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\PycharmProjects\MAGMApy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62B64F3-73E4-A744-980A-E6BCFB87624D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F200DFB1-E7F2-443F-A7BE-856620C17C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="760" windowWidth="31300" windowHeight="21240" activeTab="1" xr2:uid="{A66FC4F3-F169-E14C-B2AF-C9A0F5AF27FB}"/>
+    <workbookView xWindow="-21570" yWindow="4395" windowWidth="21615" windowHeight="16920" activeTab="3" xr2:uid="{A66FC4F3-F169-E14C-B2AF-C9A0F5AF27FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -749,9 +749,6 @@
     <t>ZnO_g</t>
   </si>
   <si>
-    <t>1*Zn, 0.5*O2</t>
-  </si>
-  <si>
     <t>ZnO_l</t>
   </si>
   <si>
@@ -765,6 +762,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>1*Zn_l, 0.5*O2</t>
   </si>
 </sst>
 </file>
@@ -1128,9 +1128,9 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1156,10 +1156,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>2655395.9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>-46992</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>-44992</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>-49586</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>-153255</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>-95362</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>-40286</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>36404</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>63948</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>204359</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>200903</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1483,13 +1483,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEBFD2C-B727-284E-A9E8-3A590E1F1B98}">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2439,13 +2439,13 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>101</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>160</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>162</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>163</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>164</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>166</v>
       </c>
@@ -3428,13 +3428,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E18122-6D19-724B-BF5D-00F815E4C0D4}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="185" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3448,13 +3448,13 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -4054,15 +4054,15 @@
         <v>-10967.931</v>
       </c>
       <c r="F36" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>95</v>
       </c>
       <c r="B37" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C37">
         <v>-12.02455</v>
@@ -4071,15 +4071,15 @@
         <v>33554.101999999999</v>
       </c>
       <c r="F37" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C38">
         <v>-5.1891999999999996</v>
@@ -4088,7 +4088,7 @@
         <v>6124.14</v>
       </c>
       <c r="F38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>